<commit_message>
adding more data and updating links
</commit_message>
<xml_diff>
--- a/Resources/Data and API Links.xlsx
+++ b/Resources/Data and API Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prisc\Documents\Fintech\Project_1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E174EFB-6754-45BA-A453-262FCE909F27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AC40F2-B1E1-43C8-9272-4687E3C34608}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25050" yWindow="3765" windowWidth="21600" windowHeight="11265" xr2:uid="{2F6F28C8-E7AB-4689-826F-E83D18A40D53}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{2F6F28C8-E7AB-4689-826F-E83D18A40D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>API</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>BLS Time Series by Month for Unemployment</t>
+  </si>
+  <si>
+    <t>https://covidtracking.com/data/national</t>
+  </si>
+  <si>
+    <t>Covidtracker - aggregated case data</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC4C14F6-F1B0-423E-B353-1456E3634C15}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,6 +645,14 @@
         <v>27</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding personal expenditure data
</commit_message>
<xml_diff>
--- a/Resources/Data and API Links.xlsx
+++ b/Resources/Data and API Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prisc\Documents\Fintech\Project_1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AC40F2-B1E1-43C8-9272-4687E3C34608}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81189DAB-0318-419F-A014-86C6498DC11B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{2F6F28C8-E7AB-4689-826F-E83D18A40D53}"/>
+    <workbookView xWindow="-28920" yWindow="1215" windowWidth="29040" windowHeight="15840" xr2:uid="{2F6F28C8-E7AB-4689-826F-E83D18A40D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>API</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>Covidtracker - aggregated case data</t>
+  </si>
+  <si>
+    <t>https://beta.bls.gov/dataViewer/view/timeseries/LNS14000000;jsessionid=B67E9E4C2185836C45B62A6FC973C7EB</t>
+  </si>
+  <si>
+    <t>BLS Time Series by Month for Unemployment 2008-2021</t>
+  </si>
+  <si>
+    <t>https://www.esrl.noaa.gov/gmd/ccgg/trends/data.html</t>
+  </si>
+  <si>
+    <t>NOAA CO2 emissions</t>
   </si>
 </sst>
 </file>
@@ -519,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC4C14F6-F1B0-423E-B353-1456E3634C15}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,6 +665,22 @@
         <v>29</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>